<commit_message>
Corrige erreur sur octave. Script gentab_all_AH
+ MAJ résultats
</commit_message>
<xml_diff>
--- a/Docs/Résultats/Résultats_30_11_15.xlsx
+++ b/Docs/Résultats/Résultats_30_11_15.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Titre</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>AH:Méthode de la banque de filtre (param=2^11)</t>
+  </si>
+  <si>
+    <t>AH: correction d'une erreur sur les bandes des octaves</t>
+  </si>
+  <si>
+    <t>Progression</t>
   </si>
 </sst>
 </file>
@@ -281,7 +287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -325,6 +331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,7 +755,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="5">
-        <v>0.86667000000000005</v>
+        <v>1</v>
       </c>
       <c r="L4" s="4">
         <v>1.6666666666666701E-2</v>
@@ -793,7 +800,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="5">
-        <v>0.91890000000000005</v>
+        <v>0.97297297297297303</v>
       </c>
       <c r="L5" s="4">
         <v>1.6666666666666701E-2</v>
@@ -838,7 +845,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="5">
-        <v>0.48709999999999998</v>
+        <v>0.487179487179487</v>
       </c>
       <c r="L6" s="4">
         <v>0</v>
@@ -928,7 +935,7 @@
         <v>0.871</v>
       </c>
       <c r="K8" s="5">
-        <v>0.72857099999999997</v>
+        <v>0.71830985915493006</v>
       </c>
       <c r="L8" s="4">
         <v>0.5</v>
@@ -973,7 +980,7 @@
         <v>0.95499999999999996</v>
       </c>
       <c r="K9" s="5">
-        <v>0.97</v>
+        <v>0.96825396825396792</v>
       </c>
       <c r="L9" s="4">
         <v>0.05</v>
@@ -1018,7 +1025,7 @@
         <v>0.90400000000000003</v>
       </c>
       <c r="K10" s="5">
-        <v>0.89200000000000002</v>
+        <v>0.97530864197530898</v>
       </c>
       <c r="L10" s="4">
         <v>0.25</v>
@@ -1060,7 +1067,7 @@
         <v>0.98699999999999999</v>
       </c>
       <c r="K11" s="5">
-        <v>0.8</v>
+        <v>0.98666666666666702</v>
       </c>
       <c r="L11" s="4">
         <v>2.5000000000000001E-2</v>
@@ -1102,7 +1109,7 @@
         <v>0.83299999999999996</v>
       </c>
       <c r="K12" s="8">
-        <v>0.83299999999999996</v>
+        <v>0.81818181818181801</v>
       </c>
       <c r="L12" s="7">
         <v>8.3333333333333297E-3</v>
@@ -1140,7 +1147,7 @@
       </c>
       <c r="K13" s="27">
         <f>SUMPRODUCT(E3:E12,K3:K12)/SUM(E3:E12)</f>
-        <v>0.82737632399299466</v>
+        <v>0.87013599220879112</v>
       </c>
       <c r="L13" s="27">
         <f>SUMPRODUCT(E3:E12,L3:L12)/SUM(E3:E12)</f>
@@ -1173,22 +1180,41 @@
       </c>
       <c r="I14" s="27"/>
       <c r="J14" s="27">
+        <v>0.97</v>
+      </c>
+      <c r="K14" s="27">
         <v>0.95</v>
-      </c>
-      <c r="K14" s="27">
-        <v>0.85</v>
       </c>
       <c r="L14" s="27">
         <v>0</v>
       </c>
       <c r="M14" s="27">
-        <v>0.95</v>
-      </c>
-      <c r="N14" s="28">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="22" spans="3:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+        <v>0.97</v>
+      </c>
+      <c r="N14" s="27">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="29">
+        <v>8.8300000000000003E-2</v>
+      </c>
+      <c r="K15" s="29">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="L20" s="4"/>
+      <c r="M20" s="3"/>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="L21" s="4"/>
+      <c r="M21" s="3"/>
+    </row>
+    <row r="22" spans="3:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C22" s="18" t="s">
         <v>20</v>
       </c>
@@ -1196,15 +1222,58 @@
         <f>SUMPRODUCT(J3:J12,E3:E12)/SUM(E3:E13)</f>
         <v>0.90958669001751313</v>
       </c>
-    </row>
-    <row r="23" spans="3:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="L22" s="4"/>
+      <c r="M22" s="3"/>
+    </row>
+    <row r="23" spans="3:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>28</v>
       </c>
+      <c r="L23" s="4"/>
+      <c r="M23" s="3"/>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+      <c r="L24" s="4"/>
+      <c r="M24" s="3"/>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="L25" s="4"/>
+      <c r="M25" s="3"/>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="L26" s="4"/>
+      <c r="M26" s="3"/>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="L27" s="4"/>
+      <c r="M27" s="3"/>
+    </row>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="L28" s="4"/>
+      <c r="M28" s="3"/>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="L29" s="4"/>
+      <c r="M29" s="3"/>
+    </row>
+    <row r="30" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+    </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F3:G13 L3:L12">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.25"/>
@@ -1216,7 +1285,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:N12 J3:K12">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0.5"/>
         <cfvo type="num" val="0.75"/>
@@ -1228,7 +1297,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H13">
-    <cfRule type="colorScale" priority="11">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="num" val="0.5"/>
         <cfvo type="num" val="0.65"/>
@@ -1240,7 +1309,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14:G14 L14">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.25"/>
@@ -1251,8 +1320,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M14:N14 J14:K14">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="J14:K14 M14:N14">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0.5"/>
         <cfvo type="num" val="0.75"/>
@@ -1264,7 +1333,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="0.5"/>
         <cfvo type="num" val="0.65"/>
@@ -1276,7 +1345,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.25"/>
@@ -1288,6 +1357,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M13:N13 J13:K13">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.75"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0"/>
+        <color rgb="FF92D050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L20:L29">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0.5"/>

</xml_diff>

<commit_message>
Améliore légèrement les résultats en fenêtrant les segments
</commit_message>
<xml_diff>
--- a/Docs/Résultats/Résultats_30_11_15.xlsx
+++ b/Docs/Résultats/Résultats_30_11_15.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Titre</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Progression</t>
+  </si>
+  <si>
+    <t>Erreur d'annotations sur No Surprises</t>
   </si>
 </sst>
 </file>
@@ -616,7 +619,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,7 +848,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="5">
-        <v>0.487179487179487</v>
+        <v>0.89700000000000002</v>
       </c>
       <c r="L6" s="4">
         <v>0</v>
@@ -1147,7 +1150,7 @@
       </c>
       <c r="K13" s="27">
         <f>SUMPRODUCT(E3:E12,K3:K12)/SUM(E3:E12)</f>
-        <v>0.87013599220879112</v>
+        <v>0.89884495983194435</v>
       </c>
       <c r="L13" s="27">
         <f>SUMPRODUCT(E3:E12,L3:L12)/SUM(E3:E12)</f>
@@ -1203,16 +1206,16 @@
         <v>8.8300000000000003E-2</v>
       </c>
       <c r="K15" s="29">
-        <v>9.6000000000000002E-2</v>
+        <v>0.12470000000000001</v>
       </c>
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="L20" s="4"/>
-      <c r="M20" s="3"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="3"/>
     </row>
     <row r="21" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="L21" s="4"/>
-      <c r="M21" s="3"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="3"/>
     </row>
     <row r="22" spans="3:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C22" s="18" t="s">
@@ -1222,8 +1225,8 @@
         <f>SUMPRODUCT(J3:J12,E3:E12)/SUM(E3:E13)</f>
         <v>0.90958669001751313</v>
       </c>
-      <c r="L22" s="4"/>
-      <c r="M22" s="3"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="3"/>
     </row>
     <row r="23" spans="3:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
@@ -1240,6 +1243,9 @@
       <c r="M24" s="3"/>
     </row>
     <row r="25" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
       <c r="L25" s="4"/>
       <c r="M25" s="3"/>
     </row>
@@ -1284,7 +1290,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:N12 J3:K12">
+  <conditionalFormatting sqref="M3:N12 J3:K12 L23:L29 K20:K22">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -1368,18 +1374,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L20:L29">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="num" val="0.5"/>
-        <cfvo type="num" val="0.75"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFFF0000"/>
-        <color theme="0"/>
-        <color rgb="FF92D050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>